<commit_message>
adding .net 9 to Console and Blazor project. Setting multitarget framework to Wpf project, with .net8 and .net 9
</commit_message>
<xml_diff>
--- a/Src/DetailedSamples/Samples/Annotations/Output/AddComment.xlsx
+++ b/Src/DetailedSamples/Samples/Annotations/Output/AddComment.xlsx
@@ -2,11 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <bookViews>
-    <workbookView xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" activeTab="1" firstSheet="0"/>
+    <workbookView xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="Rb2a523762b5c404b"/>
-    <sheet name="Xceed Trial License" sheetId="2" r:id="R1e1daa5540a644fd"/>
+    <sheet name="Sheet1" sheetId="1" r:id="R3d0dae25c10d45fb"/>
   </sheets>
 </workbook>
 </file>
@@ -14,7 +13,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>tc={cfb16d4a-8685-4f72-96f9-f493e5b87bc0}</author>
+    <author>tc={644324d3-c108-4fcf-92cf-75092abf3ed0}</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0">
@@ -27,22 +26,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t xml:space="preserve">Add Comment</t>
   </si>
-  <si>
-    <t xml:space="preserve">This workbook was created using the trial version of Xceed Workbooks for .NET.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please contact sales@xceed.com if you are ready to purchase.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <color theme="1"/>
       <sz val="11"/>
@@ -52,12 +45,6 @@
       <b/>
       <color theme="1"/>
       <sz val="15.5"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FFFF8C00"/>
-      <sz val="16"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -81,10 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="0">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -96,7 +82,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments">
-  <person displayName="ACER" id="{5a51917f-45f1-4e15-858a-cfe93b59215a}"/>
+  <person displayName="ACER" id="{9fc8e7ef-4d42-4a6f-b8d6-167fc93a5d7f}"/>
 </personList>
 </file>
 
@@ -363,16 +349,16 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments">
-  <threadedComment ref="B3" id="{cfb16d4a-8685-4f72-96f9-f493e5b87bc0}" personId="{5a51917f-45f1-4e15-858a-cfe93b59215a}" dT="2024-07-16T13:03:38.03">
+  <threadedComment ref="B3" id="{644324d3-c108-4fcf-92cf-75092abf3ed0}" personId="{9fc8e7ef-4d42-4a6f-b8d6-167fc93a5d7f}" dT="2024-10-02T17:26:39.55">
     <text>This is the title of the document.</text>
   </threadedComment>
-  <threadedComment ref="B3" id="{39b4d0dd-1851-4b7d-8d85-1e18cc1b51a9}" personId="{5a51917f-45f1-4e15-858a-cfe93b59215a}" dT="2024-07-16T13:03:38.04" parentId="{cfb16d4a-8685-4f72-96f9-f493e5b87bc0}">
+  <threadedComment ref="B3" id="{57f49758-9085-4203-a26b-3acc4634794b}" personId="{9fc8e7ef-4d42-4a6f-b8d6-167fc93a5d7f}" dT="2024-10-02T17:26:39.56" parentId="{644324d3-c108-4fcf-92cf-75092abf3ed0}">
     <text>I added another comment by mistake.</text>
   </threadedComment>
-  <threadedComment ref="B3" id="{557c575c-4d4a-4380-b9c4-b5a4f2d304f5}" personId="{5a51917f-45f1-4e15-858a-cfe93b59215a}" dT="2024-07-16T13:03:38.05" parentId="{cfb16d4a-8685-4f72-96f9-f493e5b87bc0}">
+  <threadedComment ref="B3" id="{25d5d1e0-df59-45b7-bb97-ea4cc48aace1}" personId="{9fc8e7ef-4d42-4a6f-b8d6-167fc93a5d7f}" dT="2024-10-02T17:26:39.57" parentId="{644324d3-c108-4fcf-92cf-75092abf3ed0}">
     <text>Wait I can also be in the thread of the conversation ?</text>
   </threadedComment>
-  <threadedComment ref="B3" id="{f3e8fec5-6c59-4be2-a291-c22a3535a949}" personId="{5a51917f-45f1-4e15-858a-cfe93b59215a}" dT="2024-07-16T13:03:38.06" parentId="{cfb16d4a-8685-4f72-96f9-f493e5b87bc0}">
+  <threadedComment ref="B3" id="{35de8374-fca5-4e50-96b5-af69b5725b28}" personId="{9fc8e7ef-4d42-4a6f-b8d6-167fc93a5d7f}" dT="2024-10-02T17:26:39.58" parentId="{644324d3-c108-4fcf-92cf-75092abf3ed0}">
     <text>I made another mistake but looks like I will be at the end of the thread.</text>
   </threadedComment>
 </ThreadedComments>
@@ -393,24 +379,4 @@
   </sheetData>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
 </file>
</xml_diff>